<commit_message>
Add latest ONS deaths data
</commit_message>
<xml_diff>
--- a/data/ons-deaths/explore/estimate_ewd_2020_21.xlsx
+++ b/data/ons-deaths/explore/estimate_ewd_2020_21.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24131"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu\home\mike\projects\work\covid-stats\data\ons-deaths\explore\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CE0D9C7-FD07-4888-BDCF-3FE1F1EA2F31}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C0EE0A4-6807-4F59-8B76-3C5BCEFF6C31}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="10">
   <si>
     <t>week_ended</t>
   </si>
@@ -40,13 +40,16 @@
     <t>covid_occurrences</t>
   </si>
   <si>
-    <t>EWD</t>
-  </si>
-  <si>
     <t>occ vs reg</t>
   </si>
   <si>
     <t>Jan total deaths</t>
+  </si>
+  <si>
+    <t>reg</t>
+  </si>
+  <si>
+    <t>occ</t>
   </si>
 </sst>
 </file>
@@ -554,7 +557,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
@@ -564,9 +567,7 @@
     <xf numFmtId="14" fontId="0" fillId="35" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="36" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="16" fillId="36" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
@@ -923,10 +924,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K1128"/>
+  <dimension ref="A1:K1130"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1084" workbookViewId="0">
-      <selection activeCell="J1103" sqref="J1103"/>
+    <sheetView tabSelected="1" topLeftCell="A1106" workbookViewId="0">
+      <selection activeCell="A1109" sqref="A1109"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -22786,7 +22787,7 @@
         <v>-1055</v>
       </c>
       <c r="K1092" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="1093" spans="1:11" x14ac:dyDescent="0.25">
@@ -22891,7 +22892,7 @@
       <c r="H1097" s="5">
         <v>1</v>
       </c>
-      <c r="I1097" s="10">
+      <c r="I1097" s="9">
         <f>D1097/7*H1097</f>
         <v>2122.8571428571427</v>
       </c>
@@ -22907,20 +22908,20 @@
         <v>17751</v>
       </c>
       <c r="D1098" s="5">
-        <v>16339</v>
+        <v>16330</v>
       </c>
       <c r="E1098" s="5">
         <v>6057</v>
       </c>
       <c r="F1098" s="5">
-        <v>6143</v>
+        <v>6158</v>
       </c>
       <c r="H1098" s="5">
         <v>7</v>
       </c>
-      <c r="I1098" s="10">
+      <c r="I1098" s="9">
         <f t="shared" ref="I1098:I1102" si="0">D1098/7*H1098</f>
-        <v>16339.000000000002</v>
+        <v>16329.999999999998</v>
       </c>
     </row>
     <row r="1099" spans="1:11" x14ac:dyDescent="0.25">
@@ -22934,20 +22935,20 @@
         <v>18042</v>
       </c>
       <c r="D1099" s="5">
-        <v>18423</v>
+        <v>18392</v>
       </c>
       <c r="E1099" s="5">
         <v>7245</v>
       </c>
       <c r="F1099" s="5">
-        <v>8163</v>
+        <v>8183</v>
       </c>
       <c r="H1099" s="5">
         <v>7</v>
       </c>
-      <c r="I1099" s="10">
+      <c r="I1099" s="9">
         <f t="shared" si="0"/>
-        <v>18423</v>
+        <v>18392</v>
       </c>
     </row>
     <row r="1100" spans="1:11" x14ac:dyDescent="0.25">
@@ -22961,20 +22962,20 @@
         <v>18676</v>
       </c>
       <c r="D1100" s="5">
-        <v>19180</v>
+        <v>19132</v>
       </c>
       <c r="E1100" s="5">
         <v>8422</v>
       </c>
       <c r="F1100" s="5">
-        <v>9019</v>
+        <v>9041</v>
       </c>
       <c r="H1100" s="5">
         <v>7</v>
       </c>
-      <c r="I1100" s="10">
+      <c r="I1100" s="9">
         <f t="shared" si="0"/>
-        <v>19180</v>
+        <v>19132</v>
       </c>
     </row>
     <row r="1101" spans="1:11" x14ac:dyDescent="0.25">
@@ -22988,20 +22989,20 @@
         <v>18448</v>
       </c>
       <c r="D1101" s="5">
-        <v>17911</v>
+        <v>17846</v>
       </c>
       <c r="E1101" s="5">
         <v>8433</v>
       </c>
       <c r="F1101" s="5">
-        <v>7954</v>
+        <v>7971</v>
       </c>
       <c r="H1101" s="5">
         <v>7</v>
       </c>
-      <c r="I1101" s="10">
+      <c r="I1101" s="9">
         <f t="shared" si="0"/>
-        <v>17911</v>
+        <v>17846</v>
       </c>
     </row>
     <row r="1102" spans="1:11" x14ac:dyDescent="0.25">
@@ -23015,20 +23016,20 @@
         <v>17192</v>
       </c>
       <c r="D1102" s="5">
-        <v>15768</v>
+        <v>15719</v>
       </c>
       <c r="E1102" s="5">
         <v>7320</v>
       </c>
       <c r="F1102" s="5">
-        <v>6165</v>
+        <v>6174</v>
       </c>
       <c r="H1102" s="5">
         <v>2</v>
       </c>
-      <c r="I1102" s="10">
+      <c r="I1102" s="9">
         <f t="shared" si="0"/>
-        <v>4505.1428571428569</v>
+        <v>4491.1428571428569</v>
       </c>
     </row>
     <row r="1103" spans="1:11" x14ac:dyDescent="0.25">
@@ -23042,20 +23043,20 @@
         <v>15354</v>
       </c>
       <c r="D1103" s="5">
-        <v>13903</v>
+        <v>13844</v>
       </c>
       <c r="E1103" s="5">
         <v>5691</v>
       </c>
       <c r="F1103" s="5">
-        <v>4601</v>
-      </c>
-      <c r="I1103" s="10">
+        <v>4614</v>
+      </c>
+      <c r="I1103" s="9">
         <f>SUM(I1097:I1102)</f>
-        <v>78481</v>
+        <v>78314</v>
       </c>
       <c r="J1103" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="1104" spans="1:11" x14ac:dyDescent="0.25">
@@ -23069,13 +23070,13 @@
         <v>13809</v>
       </c>
       <c r="D1104" s="5">
-        <v>13317</v>
+        <v>13290</v>
       </c>
       <c r="E1104" s="5">
         <v>4079</v>
       </c>
       <c r="F1104" s="5">
-        <v>3480</v>
+        <v>3495</v>
       </c>
     </row>
     <row r="1105" spans="1:11" x14ac:dyDescent="0.25">
@@ -23089,13 +23090,13 @@
         <v>12614</v>
       </c>
       <c r="D1105" s="5">
-        <v>11689</v>
+        <v>11664</v>
       </c>
       <c r="E1105" s="5">
         <v>2914</v>
       </c>
       <c r="F1105" s="5">
-        <v>2379</v>
+        <v>2390</v>
       </c>
     </row>
     <row r="1106" spans="1:11" x14ac:dyDescent="0.25">
@@ -23109,13 +23110,13 @@
         <v>11592</v>
       </c>
       <c r="D1106" s="5">
-        <v>10426</v>
+        <v>10420</v>
       </c>
       <c r="E1106" s="5">
         <v>2105</v>
       </c>
       <c r="F1106" s="5">
-        <v>1627</v>
+        <v>1633</v>
       </c>
     </row>
     <row r="1107" spans="1:11" x14ac:dyDescent="0.25">
@@ -23129,13 +23130,13 @@
         <v>10987</v>
       </c>
       <c r="D1107" s="5">
-        <v>10394</v>
+        <v>10367</v>
       </c>
       <c r="E1107" s="5">
         <v>1501</v>
       </c>
       <c r="F1107" s="5">
-        <v>1129</v>
+        <v>1134</v>
       </c>
     </row>
     <row r="1108" spans="1:11" x14ac:dyDescent="0.25">
@@ -23149,13 +23150,13 @@
         <v>10311</v>
       </c>
       <c r="D1108" s="5">
-        <v>9867</v>
+        <v>9853</v>
       </c>
       <c r="E1108" s="5">
         <v>963</v>
       </c>
       <c r="F1108" s="5">
-        <v>752</v>
+        <v>754</v>
       </c>
     </row>
     <row r="1109" spans="1:11" x14ac:dyDescent="0.25">
@@ -23169,13 +23170,13 @@
         <v>10045</v>
       </c>
       <c r="D1109" s="5">
-        <v>9632</v>
+        <v>9630</v>
       </c>
       <c r="E1109" s="5">
         <v>719</v>
       </c>
       <c r="F1109" s="5">
-        <v>561</v>
+        <v>565</v>
       </c>
       <c r="G1109">
         <f>(C1093+C1110)/2+SUM(C1094:C1109)</f>
@@ -23183,14 +23184,14 @@
       </c>
       <c r="H1109">
         <f>SUM(D1093:D1109)</f>
-        <v>233677</v>
+        <v>233315</v>
       </c>
       <c r="J1109">
         <f>H1109-G1109</f>
-        <v>1712</v>
+        <v>1350</v>
       </c>
       <c r="K1109" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="1110" spans="1:11" x14ac:dyDescent="0.25">
@@ -23204,13 +23205,13 @@
         <v>8201</v>
       </c>
       <c r="D1110" s="7">
-        <v>9349</v>
+        <v>9353</v>
       </c>
       <c r="E1110" s="7">
         <v>400</v>
       </c>
       <c r="F1110" s="7">
-        <v>365</v>
+        <v>366</v>
       </c>
     </row>
     <row r="1111" spans="1:11" x14ac:dyDescent="0.25">
@@ -23224,13 +23225,13 @@
         <v>9098</v>
       </c>
       <c r="D1111" s="7">
-        <v>9273</v>
+        <v>9297</v>
       </c>
       <c r="E1111" s="7">
         <v>379</v>
       </c>
       <c r="F1111" s="7">
-        <v>281</v>
+        <v>284</v>
       </c>
     </row>
     <row r="1112" spans="1:11" x14ac:dyDescent="0.25">
@@ -23244,13 +23245,13 @@
         <v>10438</v>
       </c>
       <c r="D1112" s="7">
-        <v>9362</v>
+        <v>9368</v>
       </c>
       <c r="E1112" s="7">
         <v>362</v>
       </c>
       <c r="F1112" s="7">
-        <v>238</v>
+        <v>239</v>
       </c>
     </row>
     <row r="1113" spans="1:11" x14ac:dyDescent="0.25">
@@ -23264,13 +23265,13 @@
         <v>9941</v>
       </c>
       <c r="D1113" s="7">
-        <v>9451</v>
+        <v>9471</v>
       </c>
       <c r="E1113" s="7">
         <v>260</v>
       </c>
       <c r="F1113" s="7">
-        <v>192</v>
+        <v>193</v>
       </c>
     </row>
     <row r="1114" spans="1:11" x14ac:dyDescent="0.25">
@@ -23284,7 +23285,7 @@
         <v>9692</v>
       </c>
       <c r="D1114" s="7">
-        <v>9101</v>
+        <v>9112</v>
       </c>
       <c r="E1114" s="7">
         <v>205</v>
@@ -23304,13 +23305,13 @@
         <v>7986</v>
       </c>
       <c r="D1115" s="7">
-        <v>9409</v>
+        <v>9400</v>
       </c>
       <c r="E1115" s="7">
         <v>129</v>
       </c>
       <c r="F1115" s="7">
-        <v>111</v>
+        <v>112</v>
       </c>
     </row>
     <row r="1116" spans="1:11" x14ac:dyDescent="0.25">
@@ -23324,13 +23325,13 @@
         <v>10164</v>
       </c>
       <c r="D1116" s="7">
-        <v>9399</v>
+        <v>9421</v>
       </c>
       <c r="E1116" s="7">
         <v>151</v>
       </c>
       <c r="F1116" s="7">
-        <v>88</v>
+        <v>90</v>
       </c>
     </row>
     <row r="1117" spans="1:11" x14ac:dyDescent="0.25">
@@ -23344,13 +23345,13 @@
         <v>9860</v>
       </c>
       <c r="D1117" s="7">
-        <v>9271</v>
+        <v>9284</v>
       </c>
       <c r="E1117" s="7">
         <v>107</v>
       </c>
       <c r="F1117" s="7">
-        <v>67</v>
+        <v>71</v>
       </c>
     </row>
     <row r="1118" spans="1:11" x14ac:dyDescent="0.25">
@@ -23364,7 +23365,7 @@
         <v>9628</v>
       </c>
       <c r="D1118" s="7">
-        <v>9094</v>
+        <v>9096</v>
       </c>
       <c r="E1118" s="7">
         <v>95</v>
@@ -23384,13 +23385,13 @@
         <v>7778</v>
       </c>
       <c r="D1119" s="7">
-        <v>9212</v>
+        <v>9231</v>
       </c>
       <c r="E1119" s="7">
         <v>98</v>
       </c>
       <c r="F1119" s="7">
-        <v>69</v>
+        <v>70</v>
       </c>
     </row>
     <row r="1120" spans="1:11" x14ac:dyDescent="0.25">
@@ -23404,7 +23405,7 @@
         <v>10204</v>
       </c>
       <c r="D1120" s="7">
-        <v>9051</v>
+        <v>9076</v>
       </c>
       <c r="E1120" s="7">
         <v>84</v>
@@ -23424,13 +23425,13 @@
         <v>9459</v>
       </c>
       <c r="D1121" s="7">
-        <v>8843</v>
+        <v>9031</v>
       </c>
       <c r="E1121" s="7">
         <v>102</v>
       </c>
       <c r="F1121" s="7">
-        <v>75</v>
+        <v>77</v>
       </c>
     </row>
     <row r="1122" spans="1:11" x14ac:dyDescent="0.25">
@@ -23444,13 +23445,13 @@
         <v>8690</v>
       </c>
       <c r="D1122" s="7">
-        <v>8667</v>
+        <v>9057</v>
       </c>
       <c r="E1122" s="7">
         <v>99</v>
       </c>
       <c r="F1122" s="7">
-        <v>99</v>
+        <v>106</v>
       </c>
     </row>
     <row r="1123" spans="1:11" x14ac:dyDescent="0.25">
@@ -23463,15 +23464,14 @@
       <c r="C1123" s="7">
         <v>8808</v>
       </c>
-      <c r="D1123" s="11">
-        <f>D1122</f>
-        <v>8667</v>
+      <c r="D1123" s="7">
+        <v>9488</v>
       </c>
       <c r="E1123" s="7">
         <v>109</v>
       </c>
       <c r="F1123" s="7">
-        <v>100</v>
+        <v>137</v>
       </c>
     </row>
     <row r="1124" spans="1:11" x14ac:dyDescent="0.25">
@@ -23481,16 +23481,18 @@
       <c r="B1124" s="7">
         <v>27</v>
       </c>
-      <c r="C1124" s="11">
-        <f>C1123</f>
-        <v>8808</v>
-      </c>
-      <c r="D1124" s="11">
-        <f t="shared" ref="D1124:D1126" si="1">D1123</f>
-        <v>8667</v>
-      </c>
-      <c r="E1124" s="7"/>
-      <c r="F1124" s="7"/>
+      <c r="C1124" s="7">
+        <v>9752</v>
+      </c>
+      <c r="D1124" s="7">
+        <v>9617</v>
+      </c>
+      <c r="E1124" s="7">
+        <v>183</v>
+      </c>
+      <c r="F1124" s="7">
+        <v>189</v>
+      </c>
     </row>
     <row r="1125" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1125" s="6">
@@ -23499,16 +23501,18 @@
       <c r="B1125" s="7">
         <v>28</v>
       </c>
-      <c r="C1125" s="11">
-        <f t="shared" ref="C1125:C1127" si="2">C1124</f>
-        <v>8808</v>
-      </c>
-      <c r="D1125" s="11">
-        <f t="shared" si="1"/>
-        <v>8667</v>
-      </c>
-      <c r="E1125" s="7"/>
-      <c r="F1125" s="7"/>
+      <c r="C1125" s="7">
+        <v>9697</v>
+      </c>
+      <c r="D1125" s="7">
+        <v>9469</v>
+      </c>
+      <c r="E1125" s="7">
+        <v>218</v>
+      </c>
+      <c r="F1125" s="7">
+        <v>258</v>
+      </c>
     </row>
     <row r="1126" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1126" s="6">
@@ -23517,58 +23521,126 @@
       <c r="B1126" s="7">
         <v>29</v>
       </c>
-      <c r="C1126" s="11">
-        <f t="shared" si="2"/>
-        <v>8808</v>
-      </c>
-      <c r="D1126" s="11">
-        <f t="shared" si="1"/>
-        <v>8667</v>
-      </c>
-      <c r="E1126" s="7"/>
-      <c r="F1126" s="7"/>
+      <c r="C1126" s="7">
+        <v>9744</v>
+      </c>
+      <c r="D1126" s="7">
+        <v>10953</v>
+      </c>
+      <c r="E1126" s="7">
+        <v>327</v>
+      </c>
+      <c r="F1126" s="7">
+        <v>426</v>
+      </c>
       <c r="G1126">
         <f>(C1110+C1127)/2+SUM(C1111:C1126)</f>
-        <v>156674.5</v>
+        <v>160107</v>
       </c>
       <c r="H1126">
         <f>SUM(D1110:D1126)</f>
-        <v>154150</v>
+        <v>159724</v>
       </c>
       <c r="J1126">
         <f>H1126-G1126</f>
-        <v>-2524.5</v>
+        <v>-383</v>
       </c>
       <c r="K1126" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="1127" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1127" s="8">
         <v>44407</v>
       </c>
-      <c r="B1127" s="9">
+      <c r="B1127">
         <v>30</v>
       </c>
-      <c r="C1127" s="11">
-        <f t="shared" si="2"/>
-        <v>8808</v>
-      </c>
-      <c r="D1127" s="9"/>
-      <c r="E1127" s="9"/>
-      <c r="F1127" s="9"/>
+      <c r="C1127">
+        <v>10135</v>
+      </c>
+      <c r="D1127">
+        <v>9851</v>
+      </c>
+      <c r="E1127">
+        <v>404</v>
+      </c>
+      <c r="F1127">
+        <v>479</v>
+      </c>
     </row>
     <row r="1128" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="F1128" t="s">
-        <v>6</v>
-      </c>
-      <c r="G1128" s="12">
+      <c r="A1128" s="8">
+        <v>44414</v>
+      </c>
+      <c r="B1128">
+        <v>31</v>
+      </c>
+      <c r="C1128">
+        <v>10187</v>
+      </c>
+      <c r="D1128">
+        <v>9768</v>
+      </c>
+      <c r="E1128">
+        <v>527</v>
+      </c>
+      <c r="F1128">
+        <v>536</v>
+      </c>
+      <c r="G1128" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="H1128" s="10" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="1129" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1129" s="8">
+        <v>44421</v>
+      </c>
+      <c r="B1129">
+        <v>32</v>
+      </c>
+      <c r="C1129">
+        <v>10372</v>
+      </c>
+      <c r="D1129">
+        <v>9933</v>
+      </c>
+      <c r="E1129">
+        <v>571</v>
+      </c>
+      <c r="F1129">
+        <v>521</v>
+      </c>
+      <c r="G1129" s="10">
         <f>G1109-(G1092+G1126)/2</f>
-        <v>65376.75</v>
-      </c>
-      <c r="H1128" s="12">
+        <v>63660.5</v>
+      </c>
+      <c r="H1129" s="10">
         <f>H1109-(H1092+H1126)/2</f>
-        <v>68878.5</v>
+        <v>65729.5</v>
+      </c>
+    </row>
+    <row r="1130" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1130" s="8">
+        <v>44428</v>
+      </c>
+      <c r="B1130">
+        <v>33</v>
+      </c>
+      <c r="C1130">
+        <v>10013</v>
+      </c>
+      <c r="D1130">
+        <v>8986</v>
+      </c>
+      <c r="E1130">
+        <v>570</v>
+      </c>
+      <c r="F1130">
+        <v>476</v>
       </c>
     </row>
   </sheetData>

</xml_diff>